<commit_message>
First experiments completed, added results
</commit_message>
<xml_diff>
--- a/experiment/Age Predictions Combined.xlsx
+++ b/experiment/Age Predictions Combined.xlsx
@@ -136,18 +136,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,6 +410,294 @@
       <c r="C22" s="0" t="n">
         <f aca="false">A22-B22</f>
         <v>11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <f aca="false">A24-B24</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <f aca="false">A25-B25</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <f aca="false">A26-B26</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <f aca="false">A27-B27</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <f aca="false">A28-B28</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <f aca="false">A29-B29</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <f aca="false">A30-B30</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <f aca="false">A31-B31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <f aca="false">A32-B32</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <f aca="false">A33-B33</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <f aca="false">A34-B34</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <f aca="false">A35-B35</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <f aca="false">A36-B36</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <f aca="false">A37-B37</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <f aca="false">A38-B38</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <f aca="false">A39-B39</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <f aca="false">A40-B40</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <f aca="false">A41-B41</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <f aca="false">A42-B42</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <f aca="false">A43-B43</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <f aca="false">A44-B44</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <f aca="false">A45-B45</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <f aca="false">A46-B46</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <f aca="false">A47-B47</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>